<commit_message>
Code files for week 7
</commit_message>
<xml_diff>
--- a/src/tutor/data/paralympics.xlsx
+++ b/src/tutor/data/paralympics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0035-2024-tutorials/src/tutorialpkg/data_db_activity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0034-tutorials/src/tutor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160C547E-DCEE-1244-A223-2649FF3D7082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AB899F-4B28-AA47-9BBB-FD7F8E7E9122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
@@ -2792,7 +2792,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>